<commit_message>
adding new estimates (pop; alone or in combo)
</commit_message>
<xml_diff>
--- a/data/topic_lookup.xlsx
+++ b/data/topic_lookup.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27309"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sonoshah/Dropbox/pet_project/aapidata/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/temp/community_facts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B674772-31C7-CC42-A5D7-90EF778F7870}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="18800" xr2:uid="{143384BC-56DB-874C-A28B-940B17A1F7C2}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="14320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
   <si>
     <t>pop</t>
   </si>
@@ -69,9 +74,6 @@
     <t>pct_pov_senior</t>
   </si>
   <si>
-    <t>US residents, 2016</t>
-  </si>
-  <si>
     <t>Population growth 2010-2016</t>
   </si>
   <si>
@@ -235,12 +237,21 @@
   </si>
   <si>
     <t>Turnout among registered voters</t>
+  </si>
+  <si>
+    <t>pop_v2</t>
+  </si>
+  <si>
+    <t>US residents, 2016 (Alone)</t>
+  </si>
+  <si>
+    <t>US residents, 2016 (Alone or in combo)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -597,11 +608,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96CE6CD3-9383-814F-B857-D5F4E8A1423A}">
-  <dimension ref="A1:C30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -613,13 +624,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>30</v>
-      </c>
-      <c r="C1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -627,274 +638,274 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -902,43 +913,54 @@
         <v>42</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>